<commit_message>
Se crea bom piezas.
</commit_message>
<xml_diff>
--- a/admin/bomShieldBerry.xlsx
+++ b/admin/bomShieldBerry.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="84">
   <si>
     <t>Lista de materiales para SHIELDBERRY</t>
   </si>
@@ -55,10 +55,6 @@
   </si>
   <si>
     <t>Monday, August 14, 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Componentes en el diseño
-</t>
   </si>
   <si>
     <t>Categoría</t>
@@ -287,7 +283,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +303,14 @@
       <b/>
       <sz val="12"/>
       <color indexed="32"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -463,17 +467,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -527,6 +523,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,7 +814,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -828,535 +835,542 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
+      <c r="A3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25">
+        <v>41</v>
+      </c>
+      <c r="E9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="27"/>
+      <c r="G10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="10">
+        <v>5</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="10">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="10">
+        <v>5</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="10">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="10">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="10">
+        <v>2</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="10">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="22">
         <v>41</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="14">
-        <v>5</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="14">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="25">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="14">
-        <v>5</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="14">
-        <v>1</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="23" t="s">
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="10">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="10">
-        <v>2</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="23" t="s">
+      <c r="D21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="10">
+        <v>3</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="14">
-        <v>1</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="23" t="s">
+      <c r="D25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="8">
+        <v>6</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H17" s="25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="14">
-        <v>2</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="23" t="s">
+      <c r="D27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="10">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H18" s="25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="14">
-        <v>1</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="H19" s="26">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="10">
-        <v>1</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="14">
-        <v>1</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="14">
-        <v>1</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="14">
-        <v>1</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="10">
-        <v>1</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="14">
+      <c r="D28" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="10">
+        <v>1</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="10">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="10">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="10">
         <v>3</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="10">
-        <v>1</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="12">
-        <v>6</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="22" t="s">
+      <c r="C32" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="14">
-        <v>1</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="14">
-        <v>1</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="14">
-        <v>1</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="14">
-        <v>1</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="14">
-        <v>3</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="20" t="s">
+      <c r="B33" s="6">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="10">
-        <v>1</v>
-      </c>
-      <c r="C33" s="9" t="s">
+      <c r="D33" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="E33" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="21" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="A6:C6"/>
@@ -1365,12 +1379,6 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>